<commit_message>
change zone_id type to i32
</commit_message>
<xml_diff>
--- a/zone_maker/res/文竹海外-配置源.xlsx
+++ b/zone_maker/res/文竹海外-配置源.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="166">
   <si>
     <t xml:space="preserve">龙珠区服</t>
   </si>
@@ -139,6 +139,12 @@
     <t xml:space="preserve">merge_times</t>
   </si>
   <si>
+    <t xml:space="preserve">gateway_port</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http_port</t>
+  </si>
+  <si>
     <t xml:space="preserve">Brazil 01</t>
   </si>
   <si>
@@ -187,6 +193,12 @@
     <t xml:space="preserve">2023-10-23 08:39:04</t>
   </si>
   <si>
+    <t xml:space="preserve">20001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8888</t>
+  </si>
+  <si>
     <t xml:space="preserve">Brazil 08</t>
   </si>
   <si>
@@ -211,6 +223,12 @@
     <t xml:space="preserve">2023-10-30 06:18:29</t>
   </si>
   <si>
+    <t xml:space="preserve">20002</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8889</t>
+  </si>
+  <si>
     <t xml:space="preserve">Brazil 12</t>
   </si>
   <si>
@@ -235,6 +253,12 @@
     <t xml:space="preserve">2023-12-18 05:26:58</t>
   </si>
   <si>
+    <t xml:space="preserve">20003</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8890</t>
+  </si>
+  <si>
     <t xml:space="preserve">Brazil 16</t>
   </si>
   <si>
@@ -259,6 +283,12 @@
     <t xml:space="preserve">2023-12-18 04:53:19</t>
   </si>
   <si>
+    <t xml:space="preserve">20004</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8891</t>
+  </si>
+  <si>
     <t xml:space="preserve">Brazil 18</t>
   </si>
   <si>
@@ -277,6 +307,12 @@
     <t xml:space="preserve">moshen_zone_s5018</t>
   </si>
   <si>
+    <t xml:space="preserve">20005</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8892</t>
+  </si>
+  <si>
     <t xml:space="preserve">Brazil 19</t>
   </si>
   <si>
@@ -295,6 +331,12 @@
     <t xml:space="preserve">moshen_zone_s5019</t>
   </si>
   <si>
+    <t xml:space="preserve">20006</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8893</t>
+  </si>
+  <si>
     <t xml:space="preserve">Brazil 20</t>
   </si>
   <si>
@@ -313,6 +355,12 @@
     <t xml:space="preserve">moshen_zone_s5020</t>
   </si>
   <si>
+    <t xml:space="preserve">20007</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8894</t>
+  </si>
+  <si>
     <t xml:space="preserve">Brazil 21</t>
   </si>
   <si>
@@ -331,6 +379,12 @@
     <t xml:space="preserve">moshen_zone_s5021</t>
   </si>
   <si>
+    <t xml:space="preserve">20008</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8895</t>
+  </si>
+  <si>
     <t xml:space="preserve">Brazil 22</t>
   </si>
   <si>
@@ -349,6 +403,12 @@
     <t xml:space="preserve">moshen_zone_s5022</t>
   </si>
   <si>
+    <t xml:space="preserve">20009</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8896</t>
+  </si>
+  <si>
     <t xml:space="preserve">Brazil 23</t>
   </si>
   <si>
@@ -365,6 +425,12 @@
   </si>
   <si>
     <t xml:space="preserve">moshen_zone_s5023</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20010</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8897</t>
   </si>
   <si>
     <t xml:space="preserve">http端口号：</t>
@@ -797,10 +863,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:S30"/>
+  <dimension ref="A1:U30"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="L1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="S4" activeCellId="0" sqref="S4:S8"/>
+      <selection pane="topLeft" activeCell="U4" activeCellId="0" sqref="U4:U13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -954,6 +1020,12 @@
       <c r="S3" s="3" t="s">
         <v>38</v>
       </c>
+      <c r="T3" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="U3" s="2" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="n">
@@ -963,55 +1035,61 @@
         <v>5001</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="G4" s="9" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="H4" s="9" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="K4" s="10" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="M4" s="2" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="N4" s="2" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="O4" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="P4" s="2" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="Q4" s="2" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="R4" s="2" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="S4" s="12" t="n">
         <v>1</v>
+      </c>
+      <c r="T4" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="U4" s="2" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1022,55 +1100,61 @@
         <v>5008</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="K5" s="10" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="M5" s="2" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="N5" s="2" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="O5" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="P5" s="2" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="Q5" s="2" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="R5" s="2" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="S5" s="12" t="n">
         <v>1</v>
+      </c>
+      <c r="T5" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="U5" s="2" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1081,55 +1165,61 @@
         <v>5012</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="K6" s="10" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="M6" s="2" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="N6" s="2" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="O6" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="P6" s="2" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="Q6" s="2" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="R6" s="2" t="s">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="S6" s="12" t="n">
         <v>1</v>
+      </c>
+      <c r="T6" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="U6" s="2" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1140,55 +1230,61 @@
         <v>5016</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>71</v>
+        <v>79</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>72</v>
+        <v>80</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>73</v>
+        <v>81</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>75</v>
+        <v>83</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="K7" s="10" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="L7" s="2" t="s">
-        <v>76</v>
+        <v>84</v>
       </c>
       <c r="M7" s="2" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="N7" s="2" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="O7" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="P7" s="2" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="Q7" s="2" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="R7" s="2" t="s">
-        <v>78</v>
+        <v>86</v>
       </c>
       <c r="S7" s="12" t="n">
         <v>1</v>
+      </c>
+      <c r="T7" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="U7" s="2" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1199,51 +1295,57 @@
         <v>5018</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>79</v>
+        <v>89</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="F8" s="9" t="s">
-        <v>81</v>
+        <v>91</v>
       </c>
       <c r="G8" s="13" t="s">
-        <v>82</v>
+        <v>92</v>
       </c>
       <c r="H8" s="13" t="s">
-        <v>83</v>
+        <v>93</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="K8" s="10" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="L8" s="2" t="s">
-        <v>84</v>
+        <v>94</v>
       </c>
       <c r="M8" s="2" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="N8" s="2" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="O8" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="P8" s="2" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="R8" s="1"/>
       <c r="S8" s="12" t="n">
         <v>1</v>
       </c>
+      <c r="T8" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="U8" s="2" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="n">
@@ -1253,49 +1355,55 @@
         <v>5019</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>85</v>
+        <v>97</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>86</v>
+        <v>98</v>
       </c>
       <c r="F9" s="9" t="s">
-        <v>87</v>
+        <v>99</v>
       </c>
       <c r="G9" s="13" t="s">
-        <v>88</v>
+        <v>100</v>
       </c>
       <c r="H9" s="13" t="s">
-        <v>89</v>
+        <v>101</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="K9" s="10" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="L9" s="2" t="s">
-        <v>90</v>
+        <v>102</v>
       </c>
       <c r="M9" s="2" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="N9" s="2" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="O9" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="P9" s="2" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="S9" s="12" t="n">
         <v>0</v>
+      </c>
+      <c r="T9" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="U9" s="2" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1306,49 +1414,55 @@
         <v>5020</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>91</v>
+        <v>105</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>92</v>
+        <v>106</v>
       </c>
       <c r="F10" s="9" t="s">
-        <v>93</v>
+        <v>107</v>
       </c>
       <c r="G10" s="13" t="s">
-        <v>94</v>
+        <v>108</v>
       </c>
       <c r="H10" s="13" t="s">
-        <v>95</v>
+        <v>109</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="K10" s="10" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="L10" s="2" t="s">
-        <v>96</v>
+        <v>110</v>
       </c>
       <c r="M10" s="2" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="N10" s="2" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="O10" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="P10" s="2" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="S10" s="12" t="n">
         <v>0</v>
+      </c>
+      <c r="T10" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="U10" s="2" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1359,49 +1473,55 @@
         <v>5021</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>97</v>
+        <v>113</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>98</v>
+        <v>114</v>
       </c>
       <c r="F11" s="9" t="s">
-        <v>99</v>
+        <v>115</v>
       </c>
       <c r="G11" s="13" t="s">
-        <v>100</v>
+        <v>116</v>
       </c>
       <c r="H11" s="13" t="s">
-        <v>101</v>
+        <v>117</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="K11" s="10" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="L11" s="2" t="s">
-        <v>102</v>
+        <v>118</v>
       </c>
       <c r="M11" s="2" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="N11" s="2" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="O11" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="P11" s="2" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="S11" s="12" t="n">
         <v>0</v>
+      </c>
+      <c r="T11" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="U11" s="2" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1412,49 +1532,55 @@
         <v>5022</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>103</v>
+        <v>121</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>104</v>
+        <v>122</v>
       </c>
       <c r="F12" s="9" t="s">
-        <v>105</v>
+        <v>123</v>
       </c>
       <c r="G12" s="13" t="s">
-        <v>106</v>
+        <v>124</v>
       </c>
       <c r="H12" s="13" t="s">
-        <v>107</v>
+        <v>125</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="K12" s="10" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="L12" s="2" t="s">
-        <v>108</v>
+        <v>126</v>
       </c>
       <c r="M12" s="2" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="N12" s="2" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="O12" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="P12" s="2" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="S12" s="12" t="n">
         <v>0</v>
+      </c>
+      <c r="T12" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="U12" s="2" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1465,64 +1591,70 @@
         <v>5023</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>109</v>
+        <v>129</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>110</v>
+        <v>130</v>
       </c>
       <c r="F13" s="9" t="s">
-        <v>111</v>
+        <v>131</v>
       </c>
       <c r="G13" s="13" t="s">
-        <v>112</v>
+        <v>132</v>
       </c>
       <c r="H13" s="13" t="s">
-        <v>113</v>
+        <v>133</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="K13" s="10" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="L13" s="2" t="s">
-        <v>114</v>
+        <v>134</v>
       </c>
       <c r="M13" s="2" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="N13" s="2" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="O13" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="P13" s="2" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="S13" s="12" t="n">
         <v>0</v>
       </c>
+      <c r="T13" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="U13" s="2" t="s">
+        <v>136</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="12" t="s">
-        <v>115</v>
+        <v>137</v>
       </c>
       <c r="B16" s="12"/>
       <c r="C16" s="12" t="s">
-        <v>116</v>
+        <v>138</v>
       </c>
       <c r="D16" s="12" t="s">
-        <v>117</v>
+        <v>139</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>118</v>
+        <v>140</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1535,7 +1667,7 @@
         <v>10002</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>119</v>
+        <v>141</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1547,19 +1679,19 @@
     </row>
     <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="12" t="s">
-        <v>120</v>
+        <v>142</v>
       </c>
       <c r="B19" s="12" t="s">
-        <v>121</v>
+        <v>143</v>
       </c>
       <c r="C19" s="12" t="s">
-        <v>116</v>
+        <v>138</v>
       </c>
       <c r="D19" s="12" t="s">
-        <v>117</v>
+        <v>139</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>118</v>
+        <v>140</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1567,7 +1699,7 @@
         <v>1001</v>
       </c>
       <c r="B20" s="15" t="s">
-        <v>122</v>
+        <v>144</v>
       </c>
       <c r="C20" s="15" t="n">
         <v>20011</v>
@@ -1576,7 +1708,7 @@
         <v>20021</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>123</v>
+        <v>145</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1584,7 +1716,7 @@
         <v>1002</v>
       </c>
       <c r="B21" s="15" t="s">
-        <v>124</v>
+        <v>146</v>
       </c>
       <c r="C21" s="15" t="n">
         <v>20012</v>
@@ -1593,7 +1725,7 @@
         <v>20022</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>125</v>
+        <v>147</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1601,7 +1733,7 @@
         <v>1003</v>
       </c>
       <c r="B22" s="16" t="s">
-        <v>126</v>
+        <v>148</v>
       </c>
       <c r="C22" s="17" t="n">
         <v>20013</v>
@@ -1610,7 +1742,7 @@
         <v>20023</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>127</v>
+        <v>149</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1618,7 +1750,7 @@
         <v>1004</v>
       </c>
       <c r="B23" s="15" t="s">
-        <v>128</v>
+        <v>150</v>
       </c>
       <c r="C23" s="15" t="n">
         <v>20014</v>
@@ -1627,7 +1759,7 @@
         <v>20024</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>129</v>
+        <v>151</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1635,7 +1767,7 @@
         <v>1005</v>
       </c>
       <c r="B24" s="15" t="s">
-        <v>130</v>
+        <v>152</v>
       </c>
       <c r="C24" s="15" t="n">
         <v>20015</v>
@@ -1644,7 +1776,7 @@
         <v>20025</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>131</v>
+        <v>153</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1652,7 +1784,7 @@
         <v>1006</v>
       </c>
       <c r="B25" s="15" t="s">
-        <v>132</v>
+        <v>154</v>
       </c>
       <c r="C25" s="15" t="n">
         <v>20016</v>
@@ -1661,7 +1793,7 @@
         <v>20026</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>133</v>
+        <v>155</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1669,7 +1801,7 @@
         <v>1010</v>
       </c>
       <c r="B26" s="15" t="s">
-        <v>134</v>
+        <v>156</v>
       </c>
       <c r="C26" s="15" t="n">
         <v>20017</v>
@@ -1678,7 +1810,7 @@
         <v>20027</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>135</v>
+        <v>157</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1686,7 +1818,7 @@
         <v>1008</v>
       </c>
       <c r="B27" s="15" t="s">
-        <v>136</v>
+        <v>158</v>
       </c>
       <c r="C27" s="15" t="n">
         <v>20018</v>
@@ -1695,7 +1827,7 @@
         <v>20028</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>137</v>
+        <v>159</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1703,7 +1835,7 @@
         <v>1012</v>
       </c>
       <c r="B28" s="16" t="s">
-        <v>138</v>
+        <v>160</v>
       </c>
       <c r="C28" s="17" t="n">
         <v>20019</v>
@@ -1712,7 +1844,7 @@
         <v>20029</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>139</v>
+        <v>161</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1720,7 +1852,7 @@
         <v>1013</v>
       </c>
       <c r="B29" s="18" t="s">
-        <v>140</v>
+        <v>162</v>
       </c>
       <c r="C29" s="18" t="n">
         <v>30011</v>
@@ -1729,10 +1861,10 @@
         <v>30021</v>
       </c>
       <c r="E29" s="19" t="s">
-        <v>141</v>
+        <v>163</v>
       </c>
       <c r="F29" s="20" t="s">
-        <v>142</v>
+        <v>164</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1740,7 +1872,7 @@
         <v>1014</v>
       </c>
       <c r="B30" s="18" t="s">
-        <v>140</v>
+        <v>162</v>
       </c>
       <c r="C30" s="18" t="n">
         <v>30012</v>
@@ -1749,10 +1881,10 @@
         <v>30022</v>
       </c>
       <c r="E30" s="19" t="s">
-        <v>143</v>
+        <v>165</v>
       </c>
       <c r="F30" s="20" t="s">
-        <v>142</v>
+        <v>164</v>
       </c>
     </row>
   </sheetData>

</xml_diff>